<commit_message>
vuong edit file risk_management
</commit_message>
<xml_diff>
--- a/Docs/Report1_Software requirement Specs + Project Plan_17052017/TOS_RiskManagement_v1.0_EN.xlsx
+++ b/Docs/Report1_Software requirement Specs + Project Plan_17052017/TOS_RiskManagement_v1.0_EN.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linherest/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12735" windowHeight="3975" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Guideline" sheetId="4" r:id="rId1"/>
@@ -54,11 +59,19 @@
     <definedName name="R_83">#REF!</definedName>
     <definedName name="R_84">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="rau - Personal View" guid="{76BCA86B-7D30-4D0C-A3AD-F5EB7D88CCD8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="464" activeSheetId="1"/>
     <customWorkbookView name="hanght - Personal View" guid="{6AAB2365-435B-4727-BB0B-AAE57F204611}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1012" windowHeight="571" activeSheetId="1"/>
-    <customWorkbookView name="rau - Personal View" guid="{76BCA86B-7D30-4D0C-A3AD-F5EB7D88CCD8}" mergeInterval="0" personalView="1" maximized="1" windowWidth="796" windowHeight="464" activeSheetId="1"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -69,6 +82,7 @@
     <author>MaiNTB</author>
     <author>Rod Fergusson</author>
     <author>Use</author>
+    <author>Linh Lương</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0">
@@ -402,6 +416,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="D4" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Có thể thay bằng Risk: nguồn lực JP của team có giới hạn. VD toàn N3 hết. 
+Mitigation tương ứng có thể là nhờ bạn nào N2 dịch giúp cho.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="L4" authorId="0">
       <text>
         <r>
@@ -416,6 +453,142 @@
         </r>
       </text>
     </comment>
+    <comment ref="D7" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Đọc cái này cũng chưa hiểu lắm. Có thể là muốn mô tả về việc On/Off bất thường của members nhỉ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Cái này có vẻ như là đã trở thành Issues rồi chứ ko còn là Risk nữa.
+Đang hiểu Risk ở đây có thể là: Dự án có thể ko deliver đúng hạn.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Cũng chưa hiểu lắm.
+Có thể Risk muốn mô tả ở đây là: Req chưa được chốt trc khi start dự án. 
+Mitigation tương ứng có thể là: đặt ra deadline cho KH ngày chốt Req</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Đang hiểu Risk ở đây là: Duration ngắn.
+Mitigation có thể là add thêm người -or- xin giảm scope.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Cái này hình như là Issues chứ ko còn là Risk nữa.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="4">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Linh Lương:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Cái này hình như là Issues chứ ko còn là Risk nữa.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1969,7 +2142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2133,6 +2306,31 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2182,7 +2380,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -2192,7 +2390,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -2203,26 +2401,26 @@
       <right/>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -2231,38 +2429,38 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2271,66 +2469,66 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -2338,85 +2536,85 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2424,7 +2622,7 @@
       <left/>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -2433,23 +2631,23 @@
       <left/>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2457,7 +2655,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -2465,86 +2663,88 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2921,18 +3121,99 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2942,86 +3223,17 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3032,6 +3244,36 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3041,48 +3283,6 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3102,7 +3302,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_Guideline_Process tailoring" xfId="1"/>
@@ -3470,45 +3672,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A53" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="75" customWidth="1"/>
-    <col min="2" max="2" width="2.140625" style="75" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" style="75" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="75"/>
-    <col min="5" max="5" width="13.85546875" style="75" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="75" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="75" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="75" customWidth="1"/>
-    <col min="9" max="9" width="1.7109375" style="75" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="75" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="75" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" style="75" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="75" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="75"/>
+    <col min="5" max="5" width="13.83203125" style="75" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="75" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="75" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="75" customWidth="1"/>
+    <col min="9" max="9" width="1.6640625" style="75" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="75" customWidth="1"/>
     <col min="11" max="11" width="14" style="75" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="75" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="75"/>
+    <col min="12" max="12" width="10.5" style="75" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="63" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="188" t="s">
+    <row r="1" spans="1:18" s="63" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="158" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
-      <c r="E1" s="189"/>
-      <c r="F1" s="189"/>
-      <c r="G1" s="189"/>
-      <c r="H1" s="189"/>
-      <c r="I1" s="189"/>
-      <c r="J1" s="189"/>
-      <c r="K1" s="189"/>
-      <c r="L1" s="190"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
+      <c r="J1" s="159"/>
+      <c r="K1" s="159"/>
+      <c r="L1" s="160"/>
       <c r="R1" s="64"/>
     </row>
-    <row r="2" spans="1:18" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="65"/>
       <c r="B2" s="66" t="s">
         <v>90</v>
@@ -3524,7 +3726,7 @@
       <c r="K2" s="67"/>
       <c r="L2" s="68"/>
     </row>
-    <row r="3" spans="1:18" s="69" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="69" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="70"/>
       <c r="B3" s="67"/>
       <c r="C3" s="67" t="s">
@@ -3540,7 +3742,7 @@
       <c r="K3" s="67"/>
       <c r="L3" s="68"/>
     </row>
-    <row r="4" spans="1:18" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="70"/>
       <c r="B4" s="66" t="s">
         <v>91</v>
@@ -3556,7 +3758,7 @@
       <c r="K4" s="67"/>
       <c r="L4" s="68"/>
     </row>
-    <row r="5" spans="1:18" s="69" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" s="69" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="70"/>
       <c r="B5" s="67"/>
       <c r="C5" s="67" t="s">
@@ -3572,7 +3774,7 @@
       <c r="K5" s="67"/>
       <c r="L5" s="68"/>
     </row>
-    <row r="6" spans="1:18" s="69" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" s="69" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="70"/>
       <c r="B6" s="66" t="s">
         <v>95</v>
@@ -3588,7 +3790,7 @@
       <c r="K6" s="67"/>
       <c r="L6" s="68"/>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="70"/>
       <c r="B7" s="67"/>
       <c r="C7" s="71" t="s">
@@ -3604,7 +3806,7 @@
       <c r="K7" s="73"/>
       <c r="L7" s="74"/>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="76"/>
       <c r="B8" s="73"/>
       <c r="C8" s="72" t="s">
@@ -3620,167 +3822,167 @@
       <c r="K8" s="73"/>
       <c r="L8" s="74"/>
     </row>
-    <row r="9" spans="1:18" s="80" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" s="80" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="77"/>
       <c r="B9" s="78"/>
-      <c r="C9" s="158" t="s">
+      <c r="C9" s="163" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="158"/>
-      <c r="E9" s="158"/>
-      <c r="F9" s="158"/>
-      <c r="G9" s="158"/>
-      <c r="H9" s="158"/>
-      <c r="I9" s="158"/>
-      <c r="J9" s="158"/>
-      <c r="K9" s="158"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="163"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="163"/>
+      <c r="J9" s="163"/>
+      <c r="K9" s="163"/>
       <c r="L9" s="79"/>
     </row>
-    <row r="10" spans="1:18" s="80" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" s="80" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="77"/>
       <c r="B10" s="78"/>
-      <c r="C10" s="158" t="s">
+      <c r="C10" s="163" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="158"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="158"/>
-      <c r="G10" s="158"/>
-      <c r="H10" s="158"/>
-      <c r="I10" s="158"/>
-      <c r="J10" s="158"/>
-      <c r="K10" s="158"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="163"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="163"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="163"/>
       <c r="L10" s="79"/>
     </row>
-    <row r="11" spans="1:18" s="80" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" s="80" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="77"/>
       <c r="B11" s="78"/>
-      <c r="C11" s="158" t="s">
+      <c r="C11" s="163" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="159"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="159"/>
-      <c r="G11" s="159"/>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="159"/>
+      <c r="D11" s="164"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="164"/>
+      <c r="G11" s="164"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="164"/>
+      <c r="K11" s="164"/>
       <c r="L11" s="79"/>
     </row>
-    <row r="12" spans="1:18" s="80" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" s="80" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="77"/>
       <c r="B12" s="78"/>
-      <c r="C12" s="158" t="s">
+      <c r="C12" s="163" t="s">
         <v>167</v>
       </c>
-      <c r="D12" s="159"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="159"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="159"/>
-      <c r="I12" s="159"/>
-      <c r="J12" s="159"/>
-      <c r="K12" s="159"/>
+      <c r="D12" s="164"/>
+      <c r="E12" s="164"/>
+      <c r="F12" s="164"/>
+      <c r="G12" s="164"/>
+      <c r="H12" s="164"/>
+      <c r="I12" s="164"/>
+      <c r="J12" s="164"/>
+      <c r="K12" s="164"/>
       <c r="L12" s="79"/>
     </row>
-    <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="76"/>
       <c r="B13" s="73"/>
-      <c r="C13" s="191" t="s">
+      <c r="C13" s="161" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="191"/>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191"/>
-      <c r="G13" s="191"/>
-      <c r="H13" s="191"/>
-      <c r="I13" s="191"/>
-      <c r="J13" s="191"/>
-      <c r="K13" s="191"/>
+      <c r="D13" s="161"/>
+      <c r="E13" s="161"/>
+      <c r="F13" s="161"/>
+      <c r="G13" s="161"/>
+      <c r="H13" s="161"/>
+      <c r="I13" s="161"/>
+      <c r="J13" s="161"/>
+      <c r="K13" s="161"/>
       <c r="L13" s="74"/>
     </row>
-    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="81"/>
       <c r="B14" s="82"/>
-      <c r="C14" s="184" t="s">
+      <c r="C14" s="162" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="184"/>
-      <c r="E14" s="184"/>
-      <c r="F14" s="184"/>
-      <c r="G14" s="184"/>
-      <c r="H14" s="184"/>
-      <c r="I14" s="184"/>
-      <c r="J14" s="184"/>
-      <c r="K14" s="184"/>
+      <c r="D14" s="162"/>
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="162"/>
+      <c r="I14" s="162"/>
+      <c r="J14" s="162"/>
+      <c r="K14" s="162"/>
       <c r="L14" s="74"/>
     </row>
-    <row r="15" spans="1:18" s="80" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" s="80" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="77"/>
       <c r="B15" s="78"/>
-      <c r="C15" s="158" t="s">
+      <c r="C15" s="163" t="s">
         <v>214</v>
       </c>
-      <c r="D15" s="159"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="164"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="164"/>
+      <c r="J15" s="164"/>
+      <c r="K15" s="164"/>
       <c r="L15" s="79"/>
     </row>
-    <row r="16" spans="1:18" s="80" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" s="80" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="77"/>
       <c r="B16" s="78"/>
-      <c r="C16" s="158" t="s">
+      <c r="C16" s="163" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
+      <c r="D16" s="164"/>
+      <c r="E16" s="164"/>
+      <c r="F16" s="164"/>
+      <c r="G16" s="164"/>
+      <c r="H16" s="164"/>
+      <c r="I16" s="164"/>
+      <c r="J16" s="164"/>
+      <c r="K16" s="164"/>
       <c r="L16" s="79"/>
     </row>
-    <row r="17" spans="1:12" s="80" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="80" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="77"/>
       <c r="B17" s="78"/>
-      <c r="C17" s="158" t="s">
+      <c r="C17" s="163" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="159"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
+      <c r="D17" s="164"/>
+      <c r="E17" s="164"/>
+      <c r="F17" s="164"/>
+      <c r="G17" s="164"/>
+      <c r="H17" s="164"/>
+      <c r="I17" s="164"/>
+      <c r="J17" s="164"/>
+      <c r="K17" s="164"/>
       <c r="L17" s="79"/>
     </row>
-    <row r="18" spans="1:12" s="80" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="80" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="77"/>
       <c r="B18" s="78"/>
-      <c r="C18" s="158" t="s">
+      <c r="C18" s="163" t="s">
         <v>172</v>
       </c>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="D18" s="164"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="79"/>
     </row>
-    <row r="19" spans="1:12" s="69" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="69" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="76"/>
       <c r="B19" s="66" t="s">
         <v>102</v>
@@ -3796,7 +3998,7 @@
       <c r="K19" s="67"/>
       <c r="L19" s="68"/>
     </row>
-    <row r="20" spans="1:12" s="88" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="88" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="83"/>
       <c r="B20" s="84"/>
       <c r="C20" s="85" t="s">
@@ -3812,59 +4014,59 @@
       <c r="K20" s="86"/>
       <c r="L20" s="87"/>
     </row>
-    <row r="21" spans="1:12" s="93" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="93" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="89"/>
       <c r="B21" s="90"/>
       <c r="C21" s="91" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="158" t="s">
+      <c r="D21" s="163" t="s">
         <v>173</v>
       </c>
-      <c r="E21" s="159"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
+      <c r="E21" s="164"/>
+      <c r="F21" s="164"/>
+      <c r="G21" s="164"/>
+      <c r="H21" s="164"/>
+      <c r="I21" s="164"/>
+      <c r="J21" s="164"/>
+      <c r="K21" s="164"/>
       <c r="L21" s="92"/>
     </row>
-    <row r="22" spans="1:12" s="93" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="93" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="89"/>
       <c r="B22" s="90"/>
       <c r="C22" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="158" t="s">
+      <c r="D22" s="163" t="s">
         <v>174</v>
       </c>
-      <c r="E22" s="159"/>
-      <c r="F22" s="159"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="159"/>
-      <c r="I22" s="159"/>
-      <c r="J22" s="159"/>
-      <c r="K22" s="159"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="164"/>
+      <c r="G22" s="164"/>
+      <c r="H22" s="164"/>
+      <c r="I22" s="164"/>
+      <c r="J22" s="164"/>
+      <c r="K22" s="164"/>
       <c r="L22" s="92"/>
     </row>
-    <row r="23" spans="1:12" s="93" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="93" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="89"/>
       <c r="B23" s="94"/>
       <c r="C23" s="95"/>
       <c r="D23" s="84"/>
-      <c r="E23" s="158" t="s">
+      <c r="E23" s="163" t="s">
         <v>175</v>
       </c>
-      <c r="F23" s="184"/>
-      <c r="G23" s="184"/>
-      <c r="H23" s="184"/>
-      <c r="I23" s="184"/>
-      <c r="J23" s="184"/>
-      <c r="K23" s="184"/>
+      <c r="F23" s="162"/>
+      <c r="G23" s="162"/>
+      <c r="H23" s="162"/>
+      <c r="I23" s="162"/>
+      <c r="J23" s="162"/>
+      <c r="K23" s="162"/>
       <c r="L23" s="96"/>
     </row>
-    <row r="24" spans="1:12" s="93" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="93" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="89"/>
       <c r="B24" s="94"/>
       <c r="C24" s="95"/>
@@ -3878,79 +4080,79 @@
       <c r="K24" s="98"/>
       <c r="L24" s="96"/>
     </row>
-    <row r="25" spans="1:12" s="102" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="102" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="76"/>
       <c r="B25" s="73"/>
       <c r="C25" s="99"/>
       <c r="D25" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="177" t="s">
+      <c r="E25" s="185" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="178"/>
-      <c r="G25" s="178"/>
-      <c r="H25" s="178"/>
-      <c r="I25" s="178"/>
-      <c r="J25" s="178"/>
-      <c r="K25" s="179"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="186"/>
+      <c r="H25" s="186"/>
+      <c r="I25" s="186"/>
+      <c r="J25" s="186"/>
+      <c r="K25" s="187"/>
       <c r="L25" s="101"/>
     </row>
-    <row r="26" spans="1:12" s="108" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="108" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="103"/>
       <c r="B26" s="104"/>
       <c r="C26" s="105"/>
       <c r="D26" s="106" t="s">
         <v>176</v>
       </c>
-      <c r="E26" s="180" t="s">
+      <c r="E26" s="169" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181"/>
-      <c r="I26" s="181"/>
-      <c r="J26" s="181"/>
-      <c r="K26" s="182"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="171"/>
       <c r="L26" s="107"/>
     </row>
-    <row r="27" spans="1:12" s="108" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="108" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="109"/>
       <c r="B27" s="110"/>
       <c r="C27" s="110"/>
       <c r="D27" s="111" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="180" t="s">
+      <c r="E27" s="169" t="s">
         <v>153</v>
       </c>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="181"/>
-      <c r="K27" s="182"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="170"/>
+      <c r="I27" s="170"/>
+      <c r="J27" s="170"/>
+      <c r="K27" s="171"/>
       <c r="L27" s="107"/>
     </row>
-    <row r="28" spans="1:12" s="108" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="108" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="109"/>
       <c r="B28" s="110"/>
       <c r="C28" s="112"/>
       <c r="D28" s="113" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="180" t="s">
+      <c r="E28" s="169" t="s">
         <v>177</v>
       </c>
-      <c r="F28" s="181"/>
-      <c r="G28" s="181"/>
-      <c r="H28" s="181"/>
-      <c r="I28" s="181"/>
-      <c r="J28" s="181"/>
-      <c r="K28" s="182"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="170"/>
+      <c r="I28" s="170"/>
+      <c r="J28" s="170"/>
+      <c r="K28" s="171"/>
       <c r="L28" s="107"/>
     </row>
-    <row r="29" spans="1:12" s="108" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="108" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="109"/>
       <c r="B29" s="110"/>
       <c r="C29" s="112"/>
@@ -3964,23 +4166,23 @@
       <c r="K29" s="116"/>
       <c r="L29" s="107"/>
     </row>
-    <row r="30" spans="1:12" s="93" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" s="93" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="89"/>
       <c r="B30" s="94"/>
       <c r="C30" s="95"/>
       <c r="D30" s="84"/>
-      <c r="E30" s="184" t="s">
+      <c r="E30" s="162" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="184"/>
-      <c r="G30" s="184"/>
-      <c r="H30" s="184"/>
-      <c r="I30" s="184"/>
-      <c r="J30" s="184"/>
-      <c r="K30" s="184"/>
+      <c r="F30" s="162"/>
+      <c r="G30" s="162"/>
+      <c r="H30" s="162"/>
+      <c r="I30" s="162"/>
+      <c r="J30" s="162"/>
+      <c r="K30" s="162"/>
       <c r="L30" s="96"/>
     </row>
-    <row r="31" spans="1:12" s="102" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" s="102" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="76"/>
       <c r="B31" s="73"/>
       <c r="C31" s="99"/>
@@ -3990,21 +4192,21 @@
       <c r="E31" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="165" t="s">
+      <c r="F31" s="172" t="s">
         <v>36</v>
       </c>
-      <c r="G31" s="165"/>
-      <c r="H31" s="165" t="s">
+      <c r="G31" s="172"/>
+      <c r="H31" s="172" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="165"/>
-      <c r="J31" s="165" t="s">
+      <c r="I31" s="172"/>
+      <c r="J31" s="172" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="165"/>
+      <c r="K31" s="172"/>
       <c r="L31" s="101"/>
     </row>
-    <row r="32" spans="1:12" s="123" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" s="123" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="119"/>
       <c r="B32" s="120"/>
       <c r="C32" s="120"/>
@@ -4014,21 +4216,21 @@
       <c r="E32" s="121" t="s">
         <v>116</v>
       </c>
-      <c r="F32" s="187" t="s">
+      <c r="F32" s="168" t="s">
         <v>105</v>
       </c>
-      <c r="G32" s="187"/>
-      <c r="H32" s="187" t="s">
+      <c r="G32" s="168"/>
+      <c r="H32" s="168" t="s">
         <v>107</v>
       </c>
-      <c r="I32" s="187"/>
-      <c r="J32" s="187" t="s">
+      <c r="I32" s="168"/>
+      <c r="J32" s="168" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="187"/>
+      <c r="K32" s="168"/>
       <c r="L32" s="122"/>
     </row>
-    <row r="33" spans="1:12" s="102" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="102" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="103"/>
       <c r="B33" s="104"/>
       <c r="C33" s="105"/>
@@ -4038,21 +4240,21 @@
       <c r="E33" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="187" t="s">
+      <c r="F33" s="168" t="s">
         <v>112</v>
       </c>
-      <c r="G33" s="187"/>
-      <c r="H33" s="187" t="s">
+      <c r="G33" s="168"/>
+      <c r="H33" s="168" t="s">
         <v>111</v>
       </c>
-      <c r="I33" s="187"/>
-      <c r="J33" s="187" t="s">
+      <c r="I33" s="168"/>
+      <c r="J33" s="168" t="s">
         <v>110</v>
       </c>
-      <c r="K33" s="187"/>
+      <c r="K33" s="168"/>
       <c r="L33" s="101"/>
     </row>
-    <row r="34" spans="1:12" s="102" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="102" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="103"/>
       <c r="B34" s="104"/>
       <c r="C34" s="105"/>
@@ -4062,21 +4264,21 @@
       <c r="E34" s="121" t="s">
         <v>114</v>
       </c>
-      <c r="F34" s="183" t="s">
+      <c r="F34" s="167" t="s">
         <v>113</v>
       </c>
-      <c r="G34" s="183"/>
-      <c r="H34" s="183" t="s">
+      <c r="G34" s="167"/>
+      <c r="H34" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="I34" s="183"/>
-      <c r="J34" s="183" t="s">
+      <c r="I34" s="167"/>
+      <c r="J34" s="167" t="s">
         <v>109</v>
       </c>
-      <c r="K34" s="183"/>
+      <c r="K34" s="167"/>
       <c r="L34" s="101"/>
     </row>
-    <row r="35" spans="1:12" s="69" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" s="69" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="81"/>
       <c r="B35" s="82"/>
       <c r="C35" s="67"/>
@@ -4090,23 +4292,23 @@
       <c r="K35" s="67"/>
       <c r="L35" s="124"/>
     </row>
-    <row r="36" spans="1:12" s="93" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" s="93" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="89"/>
       <c r="B36" s="94"/>
       <c r="C36" s="95"/>
       <c r="D36" s="84"/>
-      <c r="E36" s="158" t="s">
+      <c r="E36" s="163" t="s">
         <v>179</v>
       </c>
-      <c r="F36" s="184"/>
-      <c r="G36" s="184"/>
-      <c r="H36" s="184"/>
-      <c r="I36" s="184"/>
-      <c r="J36" s="184"/>
-      <c r="K36" s="184"/>
+      <c r="F36" s="162"/>
+      <c r="G36" s="162"/>
+      <c r="H36" s="162"/>
+      <c r="I36" s="162"/>
+      <c r="J36" s="162"/>
+      <c r="K36" s="162"/>
       <c r="L36" s="96"/>
     </row>
-    <row r="37" spans="1:12" s="108" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" s="108" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="76"/>
       <c r="B37" s="73"/>
       <c r="C37" s="99"/>
@@ -4120,16 +4322,16 @@
       <c r="K37" s="116"/>
       <c r="L37" s="107"/>
     </row>
-    <row r="38" spans="1:12" s="131" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="131" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A38" s="125"/>
       <c r="B38" s="126"/>
       <c r="C38" s="126"/>
       <c r="D38" s="126"/>
       <c r="E38" s="127"/>
-      <c r="F38" s="185" t="s">
+      <c r="F38" s="165" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="186"/>
+      <c r="G38" s="166"/>
       <c r="H38" s="128" t="s">
         <v>4</v>
       </c>
@@ -4138,15 +4340,15 @@
       <c r="K38" s="129"/>
       <c r="L38" s="130"/>
     </row>
-    <row r="39" spans="1:12" s="131" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="131" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A39" s="132"/>
       <c r="B39" s="129"/>
       <c r="C39" s="129"/>
       <c r="D39" s="129"/>
-      <c r="F39" s="185" t="s">
+      <c r="F39" s="165" t="s">
         <v>100</v>
       </c>
-      <c r="G39" s="186"/>
+      <c r="G39" s="166"/>
       <c r="H39" s="133" t="s">
         <v>5</v>
       </c>
@@ -4155,15 +4357,15 @@
       <c r="K39" s="129"/>
       <c r="L39" s="130"/>
     </row>
-    <row r="40" spans="1:12" s="131" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="131" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A40" s="132"/>
       <c r="B40" s="129"/>
       <c r="C40" s="129"/>
       <c r="D40" s="129"/>
-      <c r="F40" s="185" t="s">
+      <c r="F40" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="G40" s="186"/>
+      <c r="G40" s="166"/>
       <c r="H40" s="134" t="s">
         <v>32</v>
       </c>
@@ -4172,16 +4374,16 @@
       <c r="K40" s="129"/>
       <c r="L40" s="130"/>
     </row>
-    <row r="41" spans="1:12" s="127" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" s="127" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="132"/>
       <c r="B41" s="129"/>
       <c r="C41" s="129"/>
       <c r="D41" s="129"/>
       <c r="E41" s="129"/>
-      <c r="F41" s="175" t="s">
+      <c r="F41" s="183" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="176"/>
+      <c r="G41" s="184"/>
       <c r="H41" s="135" t="s">
         <v>33</v>
       </c>
@@ -4190,23 +4392,23 @@
       <c r="K41" s="126"/>
       <c r="L41" s="136"/>
     </row>
-    <row r="42" spans="1:12" s="108" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" s="108" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="109"/>
       <c r="B42" s="110"/>
       <c r="C42" s="112"/>
       <c r="D42" s="110"/>
-      <c r="E42" s="169" t="s">
+      <c r="E42" s="177" t="s">
         <v>154</v>
       </c>
-      <c r="F42" s="170"/>
-      <c r="G42" s="170"/>
-      <c r="H42" s="170"/>
-      <c r="I42" s="170"/>
-      <c r="J42" s="170"/>
-      <c r="K42" s="170"/>
+      <c r="F42" s="178"/>
+      <c r="G42" s="178"/>
+      <c r="H42" s="178"/>
+      <c r="I42" s="178"/>
+      <c r="J42" s="178"/>
+      <c r="K42" s="178"/>
       <c r="L42" s="107"/>
     </row>
-    <row r="43" spans="1:12" s="88" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" s="88" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="137"/>
       <c r="B43" s="138"/>
       <c r="C43" s="85" t="s">
@@ -4222,187 +4424,187 @@
       <c r="K43" s="86"/>
       <c r="L43" s="87"/>
     </row>
-    <row r="44" spans="1:12" s="140" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" s="140" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="139"/>
       <c r="B44" s="90"/>
       <c r="C44" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="158" t="s">
+      <c r="D44" s="163" t="s">
         <v>180</v>
       </c>
-      <c r="E44" s="159"/>
-      <c r="F44" s="159"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="159"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="159"/>
-      <c r="K44" s="159"/>
+      <c r="E44" s="164"/>
+      <c r="F44" s="164"/>
+      <c r="G44" s="164"/>
+      <c r="H44" s="164"/>
+      <c r="I44" s="164"/>
+      <c r="J44" s="164"/>
+      <c r="K44" s="164"/>
       <c r="L44" s="92"/>
     </row>
-    <row r="45" spans="1:12" s="108" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="108" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="76"/>
       <c r="B45" s="73"/>
       <c r="C45" s="99"/>
       <c r="D45" s="141" t="s">
         <v>117</v>
       </c>
-      <c r="E45" s="171" t="s">
+      <c r="E45" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="171"/>
-      <c r="G45" s="171"/>
-      <c r="H45" s="171"/>
-      <c r="I45" s="171"/>
-      <c r="J45" s="171" t="s">
+      <c r="F45" s="179"/>
+      <c r="G45" s="179"/>
+      <c r="H45" s="179"/>
+      <c r="I45" s="179"/>
+      <c r="J45" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="K45" s="171"/>
+      <c r="K45" s="179"/>
       <c r="L45" s="107"/>
     </row>
-    <row r="46" spans="1:12" s="108" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" s="108" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="109"/>
       <c r="B46" s="110"/>
       <c r="C46" s="112"/>
       <c r="D46" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="172" t="s">
+      <c r="E46" s="180" t="s">
         <v>158</v>
       </c>
-      <c r="F46" s="173"/>
-      <c r="G46" s="173"/>
-      <c r="H46" s="173"/>
-      <c r="I46" s="174"/>
-      <c r="J46" s="161" t="s">
+      <c r="F46" s="181"/>
+      <c r="G46" s="181"/>
+      <c r="H46" s="181"/>
+      <c r="I46" s="182"/>
+      <c r="J46" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="K46" s="161"/>
+      <c r="K46" s="174"/>
       <c r="L46" s="107"/>
     </row>
-    <row r="47" spans="1:12" s="69" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" s="69" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="109"/>
       <c r="B47" s="110"/>
       <c r="C47" s="112"/>
       <c r="D47" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="160" t="s">
+      <c r="E47" s="188" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="160"/>
-      <c r="G47" s="160"/>
-      <c r="H47" s="160"/>
-      <c r="I47" s="160"/>
-      <c r="J47" s="162"/>
-      <c r="K47" s="162"/>
+      <c r="F47" s="188"/>
+      <c r="G47" s="188"/>
+      <c r="H47" s="188"/>
+      <c r="I47" s="188"/>
+      <c r="J47" s="189"/>
+      <c r="K47" s="189"/>
       <c r="L47" s="68"/>
     </row>
-    <row r="48" spans="1:12" s="69" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="69" customFormat="1" ht="121.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="70"/>
       <c r="B48" s="67"/>
       <c r="C48" s="144"/>
       <c r="D48" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="160" t="s">
+      <c r="E48" s="188" t="s">
         <v>120</v>
       </c>
-      <c r="F48" s="160"/>
-      <c r="G48" s="160"/>
-      <c r="H48" s="160"/>
-      <c r="I48" s="160"/>
-      <c r="J48" s="162"/>
-      <c r="K48" s="162"/>
+      <c r="F48" s="188"/>
+      <c r="G48" s="188"/>
+      <c r="H48" s="188"/>
+      <c r="I48" s="188"/>
+      <c r="J48" s="189"/>
+      <c r="K48" s="189"/>
       <c r="L48" s="68"/>
     </row>
-    <row r="49" spans="1:12" s="108" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" s="108" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="70"/>
       <c r="B49" s="67"/>
       <c r="C49" s="144"/>
       <c r="D49" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="161" t="s">
+      <c r="E49" s="174" t="s">
         <v>50</v>
       </c>
-      <c r="F49" s="161"/>
-      <c r="G49" s="161"/>
-      <c r="H49" s="161"/>
-      <c r="I49" s="161"/>
-      <c r="J49" s="161" t="s">
+      <c r="F49" s="174"/>
+      <c r="G49" s="174"/>
+      <c r="H49" s="174"/>
+      <c r="I49" s="174"/>
+      <c r="J49" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="K49" s="161"/>
+      <c r="K49" s="174"/>
       <c r="L49" s="107"/>
     </row>
-    <row r="50" spans="1:12" s="146" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" s="146" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="89"/>
       <c r="B50" s="94"/>
       <c r="C50" s="95"/>
       <c r="D50" s="84"/>
-      <c r="E50" s="167" t="s">
+      <c r="E50" s="175" t="s">
         <v>181</v>
       </c>
-      <c r="F50" s="168"/>
-      <c r="G50" s="168"/>
-      <c r="H50" s="168"/>
-      <c r="I50" s="168"/>
-      <c r="J50" s="168"/>
-      <c r="K50" s="168"/>
+      <c r="F50" s="176"/>
+      <c r="G50" s="176"/>
+      <c r="H50" s="176"/>
+      <c r="I50" s="176"/>
+      <c r="J50" s="176"/>
+      <c r="K50" s="176"/>
       <c r="L50" s="145"/>
     </row>
-    <row r="51" spans="1:12" s="146" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" s="146" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="89"/>
       <c r="B51" s="94"/>
       <c r="C51" s="95"/>
       <c r="D51" s="84"/>
-      <c r="E51" s="163" t="s">
+      <c r="E51" s="190" t="s">
         <v>182</v>
       </c>
-      <c r="F51" s="164"/>
-      <c r="G51" s="164"/>
-      <c r="H51" s="164"/>
-      <c r="I51" s="164"/>
-      <c r="J51" s="164"/>
-      <c r="K51" s="164"/>
+      <c r="F51" s="191"/>
+      <c r="G51" s="191"/>
+      <c r="H51" s="191"/>
+      <c r="I51" s="191"/>
+      <c r="J51" s="191"/>
+      <c r="K51" s="191"/>
       <c r="L51" s="145"/>
     </row>
-    <row r="52" spans="1:12" s="149" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" s="149" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="103"/>
       <c r="B52" s="104"/>
       <c r="C52" s="105"/>
       <c r="D52" s="147"/>
-      <c r="E52" s="166" t="s">
+      <c r="E52" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="F52" s="166"/>
-      <c r="G52" s="166"/>
-      <c r="H52" s="166"/>
-      <c r="I52" s="166"/>
-      <c r="J52" s="166"/>
-      <c r="K52" s="166"/>
+      <c r="F52" s="173"/>
+      <c r="G52" s="173"/>
+      <c r="H52" s="173"/>
+      <c r="I52" s="173"/>
+      <c r="J52" s="173"/>
+      <c r="K52" s="173"/>
       <c r="L52" s="148"/>
     </row>
-    <row r="53" spans="1:12" s="140" customFormat="1" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" s="140" customFormat="1" ht="207.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="139"/>
       <c r="B53" s="90"/>
       <c r="C53" s="91" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="158" t="s">
+      <c r="D53" s="163" t="s">
         <v>183</v>
       </c>
-      <c r="E53" s="159"/>
-      <c r="F53" s="159"/>
-      <c r="G53" s="159"/>
-      <c r="H53" s="159"/>
-      <c r="I53" s="159"/>
-      <c r="J53" s="159"/>
-      <c r="K53" s="159"/>
+      <c r="E53" s="164"/>
+      <c r="F53" s="164"/>
+      <c r="G53" s="164"/>
+      <c r="H53" s="164"/>
+      <c r="I53" s="164"/>
+      <c r="J53" s="164"/>
+      <c r="K53" s="164"/>
       <c r="L53" s="92"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="150"/>
       <c r="B54" s="151"/>
       <c r="C54" s="151"/>
@@ -4418,46 +4620,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="C13:K13"/>
-    <mergeCell ref="C14:K14"/>
-    <mergeCell ref="E23:K23"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="C10:K10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="D21:K21"/>
-    <mergeCell ref="D22:K22"/>
-    <mergeCell ref="C15:K15"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="E36:K36"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="E28:K28"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="E30:K30"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C17:K17"/>
-    <mergeCell ref="C16:K16"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="E52:K52"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="D44:K44"/>
-    <mergeCell ref="E50:K50"/>
-    <mergeCell ref="E42:K42"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E45:I45"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="E25:K25"/>
     <mergeCell ref="E26:K26"/>
@@ -4470,6 +4632,46 @@
     <mergeCell ref="J48:K48"/>
     <mergeCell ref="E51:K51"/>
     <mergeCell ref="J47:K47"/>
+    <mergeCell ref="E52:K52"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="D44:K44"/>
+    <mergeCell ref="E50:K50"/>
+    <mergeCell ref="E42:K42"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E28:K28"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="E30:K30"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="E36:K36"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="C13:K13"/>
+    <mergeCell ref="C14:K14"/>
+    <mergeCell ref="E23:K23"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="C10:K10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="D21:K21"/>
+    <mergeCell ref="D22:K22"/>
+    <mergeCell ref="C15:K15"/>
+    <mergeCell ref="C17:K17"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="C18:K18"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.28000000000000003" right="0.18" top="0.38" bottom="0.63" header="0" footer="0.31"/>
@@ -4484,65 +4686,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V117"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A6"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="14" style="19" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="20" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="157" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="20" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="157" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="20" customWidth="1"/>
     <col min="11" max="11" width="8" style="19" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="19" customWidth="1"/>
+    <col min="13" max="13" width="10.1640625" style="19" customWidth="1"/>
     <col min="14" max="14" width="7" style="19" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="20" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="19"/>
-    <col min="17" max="17" width="9.28515625" style="19" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" style="20" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="19"/>
-    <col min="20" max="22" width="21.140625" style="19" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="21.140625" style="19" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" style="19" customWidth="1"/>
-    <col min="25" max="25" width="15.28515625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="17.85546875" style="19" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="19"/>
+    <col min="15" max="15" width="8.33203125" style="20" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="19"/>
+    <col min="17" max="17" width="9.33203125" style="19" customWidth="1"/>
+    <col min="18" max="18" width="8.5" style="20" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" style="19"/>
+    <col min="20" max="22" width="21.1640625" style="19" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="21.1640625" style="19" customWidth="1"/>
+    <col min="24" max="24" width="11.1640625" style="19" customWidth="1"/>
+    <col min="25" max="25" width="15.33203125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="19" customWidth="1"/>
+    <col min="27" max="16384" width="8.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="205" t="s">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="192" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
-      <c r="D1" s="205"/>
-      <c r="E1" s="205"/>
-      <c r="F1" s="205"/>
-      <c r="G1" s="205"/>
-      <c r="H1" s="205"/>
-      <c r="I1" s="205"/>
-      <c r="J1" s="205"/>
-      <c r="K1" s="205"/>
-      <c r="L1" s="205"/>
-      <c r="M1" s="205"/>
-      <c r="N1" s="205"/>
-      <c r="O1" s="205"/>
-      <c r="P1" s="205"/>
-      <c r="Q1" s="205"/>
-      <c r="R1" s="205"/>
-      <c r="S1" s="205"/>
-    </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
+      <c r="M1" s="192"/>
+      <c r="N1" s="192"/>
+      <c r="O1" s="192"/>
+      <c r="P1" s="192"/>
+      <c r="Q1" s="192"/>
+      <c r="R1" s="192"/>
+      <c r="S1" s="192"/>
+    </row>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -4552,7 +4754,7 @@
       <c r="O2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:22" s="3" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" s="3" customFormat="1" ht="33" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
@@ -4617,8 +4819,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="202" t="s">
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="55" x14ac:dyDescent="0.15">
+      <c r="A4" s="193" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="199" t="s">
@@ -4627,29 +4829,29 @@
       <c r="C4" s="199" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="202" t="s">
+      <c r="D4" s="193" t="s">
         <v>229</v>
       </c>
-      <c r="E4" s="192">
+      <c r="E4" s="196">
         <v>0.3</v>
       </c>
-      <c r="F4" s="192">
+      <c r="F4" s="196">
         <v>2</v>
       </c>
-      <c r="G4" s="192">
+      <c r="G4" s="196">
         <f>E4*F4</f>
         <v>0.6</v>
       </c>
-      <c r="H4" s="192">
+      <c r="H4" s="196">
         <v>4</v>
       </c>
-      <c r="I4" s="206" t="s">
+      <c r="I4" s="202" t="s">
         <v>230</v>
       </c>
-      <c r="J4" s="192" t="s">
+      <c r="J4" s="196" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="209"/>
+      <c r="K4" s="205"/>
       <c r="L4" s="7" t="s">
         <v>221</v>
       </c>
@@ -4672,18 +4874,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="203"/>
+    <row r="5" spans="1:22" s="2" customFormat="1" ht="33" x14ac:dyDescent="0.15">
+      <c r="A5" s="194"/>
       <c r="B5" s="200"/>
       <c r="C5" s="200"/>
-      <c r="D5" s="203"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="193"/>
-      <c r="I5" s="207"/>
-      <c r="J5" s="193"/>
-      <c r="K5" s="210"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="197"/>
+      <c r="F5" s="197"/>
+      <c r="G5" s="197"/>
+      <c r="H5" s="197"/>
+      <c r="I5" s="203"/>
+      <c r="J5" s="197"/>
+      <c r="K5" s="206"/>
       <c r="L5" s="8" t="s">
         <v>222</v>
       </c>
@@ -4706,18 +4908,18 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="2" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="204"/>
+    <row r="6" spans="1:22" s="2" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="195"/>
       <c r="B6" s="201"/>
       <c r="C6" s="201"/>
-      <c r="D6" s="204"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="208"/>
-      <c r="J6" s="194"/>
-      <c r="K6" s="211"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="198"/>
+      <c r="F6" s="198"/>
+      <c r="G6" s="198"/>
+      <c r="H6" s="198"/>
+      <c r="I6" s="204"/>
+      <c r="J6" s="198"/>
+      <c r="K6" s="207"/>
       <c r="L6" s="8" t="s">
         <v>223</v>
       </c>
@@ -4740,8 +4942,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="2" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="192" t="s">
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="196" t="s">
         <v>215</v>
       </c>
       <c r="B7" s="199" t="s">
@@ -4750,41 +4952,41 @@
       <c r="C7" s="199" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="192" t="s">
+      <c r="D7" s="196" t="s">
         <v>216</v>
       </c>
-      <c r="E7" s="192">
+      <c r="E7" s="196">
         <v>0.2</v>
       </c>
-      <c r="F7" s="192">
+      <c r="F7" s="196">
         <v>8</v>
       </c>
-      <c r="G7" s="192">
+      <c r="G7" s="196">
         <f>E7*F7</f>
         <v>1.6</v>
       </c>
-      <c r="H7" s="192">
+      <c r="H7" s="196">
         <v>3</v>
       </c>
-      <c r="I7" s="202" t="s">
+      <c r="I7" s="193" t="s">
         <v>231</v>
       </c>
-      <c r="J7" s="192" t="s">
+      <c r="J7" s="196" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="192"/>
-      <c r="L7" s="192"/>
-      <c r="M7" s="192" t="s">
+      <c r="K7" s="196"/>
+      <c r="L7" s="196"/>
+      <c r="M7" s="196" t="s">
         <v>224</v>
       </c>
-      <c r="N7" s="192" t="s">
+      <c r="N7" s="196" t="s">
         <v>234</v>
       </c>
-      <c r="O7" s="192"/>
-      <c r="P7" s="192"/>
-      <c r="Q7" s="192"/>
-      <c r="R7" s="192"/>
-      <c r="S7" s="192"/>
+      <c r="O7" s="196"/>
+      <c r="P7" s="196"/>
+      <c r="Q7" s="196"/>
+      <c r="R7" s="196"/>
+      <c r="S7" s="196"/>
       <c r="T7" s="10" t="s">
         <v>122</v>
       </c>
@@ -4795,26 +4997,26 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="193"/>
+    <row r="8" spans="1:22" s="2" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+      <c r="A8" s="197"/>
       <c r="B8" s="200"/>
       <c r="C8" s="200"/>
-      <c r="D8" s="193"/>
-      <c r="E8" s="193"/>
-      <c r="F8" s="193"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="193"/>
-      <c r="I8" s="203"/>
-      <c r="J8" s="193"/>
-      <c r="K8" s="193"/>
-      <c r="L8" s="193"/>
-      <c r="M8" s="193"/>
-      <c r="N8" s="193"/>
-      <c r="O8" s="193"/>
-      <c r="P8" s="193"/>
-      <c r="Q8" s="193"/>
-      <c r="R8" s="193"/>
-      <c r="S8" s="193"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="194"/>
+      <c r="J8" s="197"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="197"/>
+      <c r="M8" s="197"/>
+      <c r="N8" s="197"/>
+      <c r="O8" s="197"/>
+      <c r="P8" s="197"/>
+      <c r="Q8" s="197"/>
+      <c r="R8" s="197"/>
+      <c r="S8" s="197"/>
       <c r="T8" s="10" t="s">
         <v>17</v>
       </c>
@@ -4825,26 +5027,26 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="194"/>
+    <row r="9" spans="1:22" s="2" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+      <c r="A9" s="198"/>
       <c r="B9" s="201"/>
       <c r="C9" s="201"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="204"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="194"/>
-      <c r="M9" s="194"/>
-      <c r="N9" s="194"/>
-      <c r="O9" s="194"/>
-      <c r="P9" s="194"/>
-      <c r="Q9" s="194"/>
-      <c r="R9" s="194"/>
-      <c r="S9" s="194"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="198"/>
+      <c r="F9" s="198"/>
+      <c r="G9" s="198"/>
+      <c r="H9" s="198"/>
+      <c r="I9" s="195"/>
+      <c r="J9" s="198"/>
+      <c r="K9" s="198"/>
+      <c r="L9" s="198"/>
+      <c r="M9" s="198"/>
+      <c r="N9" s="198"/>
+      <c r="O9" s="198"/>
+      <c r="P9" s="198"/>
+      <c r="Q9" s="198"/>
+      <c r="R9" s="198"/>
+      <c r="S9" s="198"/>
       <c r="T9" s="10" t="s">
         <v>58</v>
       </c>
@@ -4852,8 +5054,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="192" t="s">
+    <row r="10" spans="1:22" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.15">
+      <c r="A10" s="196" t="s">
         <v>217</v>
       </c>
       <c r="B10" s="199" t="s">
@@ -4862,29 +5064,29 @@
       <c r="C10" s="199" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="192" t="s">
+      <c r="D10" s="196" t="s">
         <v>219</v>
       </c>
-      <c r="E10" s="192">
+      <c r="E10" s="196">
         <v>0.5</v>
       </c>
-      <c r="F10" s="192">
+      <c r="F10" s="196">
         <v>5</v>
       </c>
-      <c r="G10" s="192">
+      <c r="G10" s="196">
         <f>E10*F10</f>
         <v>2.5</v>
       </c>
-      <c r="H10" s="192">
+      <c r="H10" s="196">
         <v>1</v>
       </c>
-      <c r="I10" s="202" t="s">
+      <c r="I10" s="193" t="s">
         <v>233</v>
       </c>
-      <c r="J10" s="192" t="s">
+      <c r="J10" s="196" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="195"/>
+      <c r="K10" s="209"/>
       <c r="L10" s="8" t="s">
         <v>226</v>
       </c>
@@ -4904,61 +5106,61 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="2" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="193"/>
+    <row r="11" spans="1:22" s="2" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="197"/>
       <c r="B11" s="200"/>
       <c r="C11" s="200"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="193"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="203"/>
-      <c r="J11" s="193"/>
-      <c r="K11" s="196"/>
-      <c r="L11" s="192" t="s">
+      <c r="D11" s="197"/>
+      <c r="E11" s="197"/>
+      <c r="F11" s="197"/>
+      <c r="G11" s="197"/>
+      <c r="H11" s="197"/>
+      <c r="I11" s="194"/>
+      <c r="J11" s="197"/>
+      <c r="K11" s="210"/>
+      <c r="L11" s="196" t="s">
         <v>227</v>
       </c>
-      <c r="M11" s="198"/>
-      <c r="N11" s="192" t="s">
+      <c r="M11" s="208"/>
+      <c r="N11" s="196" t="s">
         <v>254</v>
       </c>
-      <c r="O11" s="198"/>
-      <c r="P11" s="198"/>
-      <c r="Q11" s="198"/>
-      <c r="R11" s="198"/>
-      <c r="S11" s="198"/>
+      <c r="O11" s="208"/>
+      <c r="P11" s="208"/>
+      <c r="Q11" s="208"/>
+      <c r="R11" s="208"/>
+      <c r="S11" s="208"/>
       <c r="T11" s="14"/>
       <c r="U11" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="2" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="194"/>
+    <row r="12" spans="1:22" s="2" customFormat="1" ht="11" x14ac:dyDescent="0.15">
+      <c r="A12" s="198"/>
       <c r="B12" s="201"/>
       <c r="C12" s="201"/>
-      <c r="D12" s="194"/>
-      <c r="E12" s="194"/>
-      <c r="F12" s="194"/>
-      <c r="G12" s="194"/>
-      <c r="H12" s="194"/>
-      <c r="I12" s="204"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="197"/>
-      <c r="L12" s="194"/>
-      <c r="M12" s="198"/>
-      <c r="N12" s="194"/>
-      <c r="O12" s="198"/>
-      <c r="P12" s="198"/>
-      <c r="Q12" s="198"/>
-      <c r="R12" s="198"/>
-      <c r="S12" s="198"/>
+      <c r="D12" s="198"/>
+      <c r="E12" s="198"/>
+      <c r="F12" s="198"/>
+      <c r="G12" s="198"/>
+      <c r="H12" s="198"/>
+      <c r="I12" s="195"/>
+      <c r="J12" s="198"/>
+      <c r="K12" s="211"/>
+      <c r="L12" s="198"/>
+      <c r="M12" s="208"/>
+      <c r="N12" s="198"/>
+      <c r="O12" s="208"/>
+      <c r="P12" s="208"/>
+      <c r="Q12" s="208"/>
+      <c r="R12" s="208"/>
+      <c r="S12" s="208"/>
       <c r="T12" s="14"/>
       <c r="U12" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="2" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>218</v>
       </c>
@@ -5008,7 +5210,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="14" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" s="14" customFormat="1" ht="44" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
         <v>235</v>
       </c>
@@ -5057,7 +5259,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="14" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" s="14" customFormat="1" ht="44" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
         <v>236</v>
       </c>
@@ -5106,7 +5308,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="14" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" s="14" customFormat="1" ht="55" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
         <v>237</v>
       </c>
@@ -5155,7 +5357,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="14" customFormat="1" ht="112.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" s="14" customFormat="1" ht="88" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>238</v>
       </c>
@@ -5204,7 +5406,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="14" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" s="14" customFormat="1" ht="66" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>239</v>
       </c>
@@ -5253,7 +5455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" s="14" customFormat="1" ht="44" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>261</v>
       </c>
@@ -5298,7 +5500,7 @@
       <c r="S19" s="8"/>
       <c r="U19" s="11"/>
     </row>
-    <row r="20" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B20" s="16"/>
       <c r="C20" s="17"/>
       <c r="E20" s="15"/>
@@ -5313,7 +5515,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B21" s="16"/>
       <c r="C21" s="17"/>
       <c r="E21" s="15"/>
@@ -5328,7 +5530,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B22" s="16"/>
       <c r="C22" s="17"/>
       <c r="E22" s="15"/>
@@ -5343,7 +5545,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="E23" s="15"/>
@@ -5358,7 +5560,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="E24" s="15"/>
@@ -5373,7 +5575,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="E25" s="15"/>
@@ -5388,7 +5590,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="E26" s="15"/>
@@ -5403,7 +5605,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="E27" s="15"/>
@@ -5418,7 +5620,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="E28" s="15"/>
@@ -5433,7 +5635,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="E29" s="15"/>
@@ -5448,7 +5650,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="E30" s="15"/>
@@ -5463,7 +5665,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="E31" s="15"/>
@@ -5478,7 +5680,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="E32" s="15"/>
@@ -5493,7 +5695,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="E33" s="15"/>
@@ -5508,7 +5710,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="E34" s="15"/>
@@ -5523,7 +5725,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="E35" s="15"/>
@@ -5538,7 +5740,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="E36" s="15"/>
@@ -5553,7 +5755,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="E37" s="15"/>
@@ -5565,7 +5767,7 @@
       <c r="O37" s="15"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="E38" s="15"/>
@@ -5577,7 +5779,7 @@
       <c r="O38" s="15"/>
       <c r="R38" s="15"/>
     </row>
-    <row r="39" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="E39" s="15"/>
@@ -5589,7 +5791,7 @@
       <c r="O39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="E40" s="15"/>
@@ -5601,7 +5803,7 @@
       <c r="O40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="E41" s="15"/>
@@ -5613,7 +5815,7 @@
       <c r="O41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="E42" s="15"/>
@@ -5625,7 +5827,7 @@
       <c r="O42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="E43" s="15"/>
@@ -5637,7 +5839,7 @@
       <c r="O43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="E44" s="15"/>
@@ -5649,7 +5851,7 @@
       <c r="O44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
       <c r="E45" s="15"/>
@@ -5661,7 +5863,7 @@
       <c r="O45" s="15"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
       <c r="E46" s="15"/>
@@ -5673,7 +5875,7 @@
       <c r="O46" s="15"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="E47" s="15"/>
@@ -5685,7 +5887,7 @@
       <c r="O47" s="15"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="2:21" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:21" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="E48" s="15"/>
@@ -5697,7 +5899,7 @@
       <c r="O48" s="15"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="E49" s="15"/>
@@ -5709,7 +5911,7 @@
       <c r="O49" s="15"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
       <c r="G50" s="15"/>
@@ -5719,7 +5921,7 @@
       <c r="O50" s="15"/>
       <c r="R50" s="15"/>
     </row>
-    <row r="51" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
       <c r="G51" s="15"/>
@@ -5729,7 +5931,7 @@
       <c r="O51" s="15"/>
       <c r="R51" s="15"/>
     </row>
-    <row r="52" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
@@ -5739,7 +5941,7 @@
       <c r="O52" s="15"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E53" s="15"/>
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
@@ -5749,7 +5951,7 @@
       <c r="O53" s="15"/>
       <c r="R53" s="15"/>
     </row>
-    <row r="54" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
@@ -5759,7 +5961,7 @@
       <c r="O54" s="15"/>
       <c r="R54" s="15"/>
     </row>
-    <row r="55" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
@@ -5769,7 +5971,7 @@
       <c r="O55" s="15"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
@@ -5779,7 +5981,7 @@
       <c r="O56" s="15"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
@@ -5789,7 +5991,7 @@
       <c r="O57" s="15"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
@@ -5799,7 +6001,7 @@
       <c r="O58" s="15"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
@@ -5809,7 +6011,7 @@
       <c r="O59" s="15"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
@@ -5819,7 +6021,7 @@
       <c r="O60" s="15"/>
       <c r="R60" s="15"/>
     </row>
-    <row r="61" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -5829,7 +6031,7 @@
       <c r="O61" s="15"/>
       <c r="R61" s="15"/>
     </row>
-    <row r="62" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
@@ -5839,7 +6041,7 @@
       <c r="O62" s="15"/>
       <c r="R62" s="15"/>
     </row>
-    <row r="63" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E63" s="15"/>
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
@@ -5849,7 +6051,7 @@
       <c r="O63" s="15"/>
       <c r="R63" s="15"/>
     </row>
-    <row r="64" spans="2:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
       <c r="G64" s="15"/>
@@ -5859,7 +6061,7 @@
       <c r="O64" s="15"/>
       <c r="R64" s="15"/>
     </row>
-    <row r="65" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
@@ -5869,7 +6071,7 @@
       <c r="O65" s="15"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E66" s="15"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
@@ -5879,7 +6081,7 @@
       <c r="O66" s="15"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E67" s="15"/>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -5889,7 +6091,7 @@
       <c r="O67" s="15"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E68" s="15"/>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
@@ -5899,7 +6101,7 @@
       <c r="O68" s="15"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
       <c r="G69" s="15"/>
@@ -5909,7 +6111,7 @@
       <c r="O69" s="15"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E70" s="15"/>
       <c r="F70" s="15"/>
       <c r="G70" s="15"/>
@@ -5919,7 +6121,7 @@
       <c r="O70" s="15"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E71" s="15"/>
       <c r="F71" s="15"/>
       <c r="G71" s="15"/>
@@ -5929,7 +6131,7 @@
       <c r="O71" s="15"/>
       <c r="R71" s="15"/>
     </row>
-    <row r="72" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E72" s="15"/>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
@@ -5939,7 +6141,7 @@
       <c r="O72" s="15"/>
       <c r="R72" s="15"/>
     </row>
-    <row r="73" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E73" s="15"/>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
@@ -5949,7 +6151,7 @@
       <c r="O73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
@@ -5959,7 +6161,7 @@
       <c r="O74" s="15"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E75" s="15"/>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
@@ -5969,7 +6171,7 @@
       <c r="O75" s="15"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E76" s="15"/>
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
@@ -5979,7 +6181,7 @@
       <c r="O76" s="15"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E77" s="15"/>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
@@ -5989,7 +6191,7 @@
       <c r="O77" s="15"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E78" s="15"/>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
@@ -5999,7 +6201,7 @@
       <c r="O78" s="15"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -6009,7 +6211,7 @@
       <c r="O79" s="15"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
@@ -6019,7 +6221,7 @@
       <c r="O80" s="15"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E81" s="15"/>
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
@@ -6029,7 +6231,7 @@
       <c r="O81" s="15"/>
       <c r="R81" s="15"/>
     </row>
-    <row r="82" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E82" s="15"/>
       <c r="F82" s="15"/>
       <c r="G82" s="15"/>
@@ -6039,7 +6241,7 @@
       <c r="O82" s="15"/>
       <c r="R82" s="15"/>
     </row>
-    <row r="83" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E83" s="15"/>
       <c r="F83" s="15"/>
       <c r="G83" s="15"/>
@@ -6049,7 +6251,7 @@
       <c r="O83" s="15"/>
       <c r="R83" s="15"/>
     </row>
-    <row r="84" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E84" s="15"/>
       <c r="F84" s="15"/>
       <c r="G84" s="15"/>
@@ -6059,7 +6261,7 @@
       <c r="O84" s="15"/>
       <c r="R84" s="15"/>
     </row>
-    <row r="85" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E85" s="15"/>
       <c r="F85" s="15"/>
       <c r="G85" s="15"/>
@@ -6069,7 +6271,7 @@
       <c r="O85" s="15"/>
       <c r="R85" s="15"/>
     </row>
-    <row r="86" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E86" s="15"/>
       <c r="F86" s="15"/>
       <c r="G86" s="15"/>
@@ -6079,7 +6281,7 @@
       <c r="O86" s="15"/>
       <c r="R86" s="15"/>
     </row>
-    <row r="87" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E87" s="15"/>
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
@@ -6089,7 +6291,7 @@
       <c r="O87" s="15"/>
       <c r="R87" s="15"/>
     </row>
-    <row r="88" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E88" s="15"/>
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
@@ -6099,7 +6301,7 @@
       <c r="O88" s="15"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E89" s="15"/>
       <c r="F89" s="15"/>
       <c r="G89" s="15"/>
@@ -6109,7 +6311,7 @@
       <c r="O89" s="15"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E90" s="15"/>
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
@@ -6119,7 +6321,7 @@
       <c r="O90" s="15"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E91" s="15"/>
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
@@ -6129,7 +6331,7 @@
       <c r="O91" s="15"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
@@ -6139,7 +6341,7 @@
       <c r="O92" s="15"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E93" s="15"/>
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
@@ -6149,7 +6351,7 @@
       <c r="O93" s="15"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E94" s="15"/>
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
@@ -6159,7 +6361,7 @@
       <c r="O94" s="15"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E95" s="15"/>
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
@@ -6169,7 +6371,7 @@
       <c r="O95" s="15"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E96" s="15"/>
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
@@ -6179,7 +6381,7 @@
       <c r="O96" s="15"/>
       <c r="R96" s="15"/>
     </row>
-    <row r="97" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E97" s="15"/>
       <c r="F97" s="15"/>
       <c r="G97" s="15"/>
@@ -6189,7 +6391,7 @@
       <c r="O97" s="15"/>
       <c r="R97" s="15"/>
     </row>
-    <row r="98" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E98" s="15"/>
       <c r="F98" s="15"/>
       <c r="G98" s="15"/>
@@ -6199,7 +6401,7 @@
       <c r="O98" s="15"/>
       <c r="R98" s="15"/>
     </row>
-    <row r="99" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E99" s="15"/>
       <c r="F99" s="15"/>
       <c r="G99" s="15"/>
@@ -6209,7 +6411,7 @@
       <c r="O99" s="15"/>
       <c r="R99" s="15"/>
     </row>
-    <row r="100" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E100" s="15"/>
       <c r="F100" s="15"/>
       <c r="G100" s="15"/>
@@ -6219,7 +6421,7 @@
       <c r="O100" s="15"/>
       <c r="R100" s="15"/>
     </row>
-    <row r="101" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E101" s="15"/>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
@@ -6229,7 +6431,7 @@
       <c r="O101" s="15"/>
       <c r="R101" s="15"/>
     </row>
-    <row r="102" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E102" s="15"/>
       <c r="F102" s="15"/>
       <c r="G102" s="15"/>
@@ -6239,7 +6441,7 @@
       <c r="O102" s="15"/>
       <c r="R102" s="15"/>
     </row>
-    <row r="103" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E103" s="15"/>
       <c r="F103" s="15"/>
       <c r="G103" s="15"/>
@@ -6249,7 +6451,7 @@
       <c r="O103" s="15"/>
       <c r="R103" s="15"/>
     </row>
-    <row r="104" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E104" s="15"/>
       <c r="F104" s="15"/>
       <c r="G104" s="15"/>
@@ -6259,7 +6461,7 @@
       <c r="O104" s="15"/>
       <c r="R104" s="15"/>
     </row>
-    <row r="105" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E105" s="15"/>
       <c r="F105" s="15"/>
       <c r="G105" s="15"/>
@@ -6269,7 +6471,7 @@
       <c r="O105" s="15"/>
       <c r="R105" s="15"/>
     </row>
-    <row r="106" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E106" s="15"/>
       <c r="F106" s="15"/>
       <c r="G106" s="15"/>
@@ -6279,7 +6481,7 @@
       <c r="O106" s="15"/>
       <c r="R106" s="15"/>
     </row>
-    <row r="107" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E107" s="15"/>
       <c r="F107" s="15"/>
       <c r="G107" s="15"/>
@@ -6289,7 +6491,7 @@
       <c r="O107" s="15"/>
       <c r="R107" s="15"/>
     </row>
-    <row r="108" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E108" s="15"/>
       <c r="F108" s="15"/>
       <c r="G108" s="15"/>
@@ -6299,7 +6501,7 @@
       <c r="O108" s="15"/>
       <c r="R108" s="15"/>
     </row>
-    <row r="109" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E109" s="15"/>
       <c r="F109" s="15"/>
       <c r="G109" s="15"/>
@@ -6309,7 +6511,7 @@
       <c r="O109" s="15"/>
       <c r="R109" s="15"/>
     </row>
-    <row r="110" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E110" s="15"/>
       <c r="F110" s="15"/>
       <c r="G110" s="15"/>
@@ -6319,7 +6521,7 @@
       <c r="O110" s="15"/>
       <c r="R110" s="15"/>
     </row>
-    <row r="111" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E111" s="15"/>
       <c r="F111" s="15"/>
       <c r="G111" s="15"/>
@@ -6329,7 +6531,7 @@
       <c r="O111" s="15"/>
       <c r="R111" s="15"/>
     </row>
-    <row r="112" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
       <c r="G112" s="15"/>
@@ -6339,7 +6541,7 @@
       <c r="O112" s="15"/>
       <c r="R112" s="15"/>
     </row>
-    <row r="113" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E113" s="15"/>
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
@@ -6349,7 +6551,7 @@
       <c r="O113" s="15"/>
       <c r="R113" s="15"/>
     </row>
-    <row r="114" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E114" s="15"/>
       <c r="F114" s="15"/>
       <c r="G114" s="15"/>
@@ -6359,7 +6561,7 @@
       <c r="O114" s="15"/>
       <c r="R114" s="15"/>
     </row>
-    <row r="115" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E115" s="15"/>
       <c r="F115" s="15"/>
       <c r="G115" s="15"/>
@@ -6369,7 +6571,7 @@
       <c r="O115" s="15"/>
       <c r="R115" s="15"/>
     </row>
-    <row r="116" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E116" s="15"/>
       <c r="F116" s="15"/>
       <c r="G116" s="15"/>
@@ -6379,7 +6581,7 @@
       <c r="O116" s="15"/>
       <c r="R116" s="15"/>
     </row>
-    <row r="117" spans="5:18" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:18" s="14" customFormat="1" ht="11" x14ac:dyDescent="0.15">
       <c r="E117" s="15"/>
       <c r="F117" s="15"/>
       <c r="G117" s="15"/>
@@ -6391,16 +6593,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6AAB2365-435B-4727-BB0B-AAE57F204611}" showRuler="0" topLeftCell="F1">
-      <selection activeCell="J14" sqref="J14"/>
+    <customSheetView guid="{76BCA86B-7D30-4D0C-A3AD-F5EB7D88CCD8}" showPageBreaks="1" showRuler="0" topLeftCell="O1">
+      <selection activeCell="R3" sqref="R3"/>
       <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0" footer="0"/>
       <pageSetup orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0">
         <oddFooter>&amp;L&amp;8 01fe-BM/PM/HDCV/FSOFT v1/0</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{76BCA86B-7D30-4D0C-A3AD-F5EB7D88CCD8}" showPageBreaks="1" showRuler="0" topLeftCell="O1">
-      <selection activeCell="R3" sqref="R3"/>
+    <customSheetView guid="{6AAB2365-435B-4727-BB0B-AAE57F204611}" showRuler="0" topLeftCell="F1">
+      <selection activeCell="J14" sqref="J14"/>
       <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.75" header="0" footer="0"/>
       <pageSetup orientation="landscape" r:id="rId2"/>
       <headerFooter alignWithMargins="0">
@@ -6409,6 +6611,40 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="50">
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="R7:R9"/>
+    <mergeCell ref="S7:S9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C4:C6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="D7:D9"/>
@@ -6425,40 +6661,6 @@
     <mergeCell ref="O7:O9"/>
     <mergeCell ref="P7:P9"/>
     <mergeCell ref="Q7:Q9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="R7:R9"/>
-    <mergeCell ref="S7:S9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="M11:M12"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="6">
@@ -6493,27 +6695,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C3" sqref="C3"/>
       <selection pane="topRight" activeCell="D3" sqref="D3"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="59" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="59" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="59" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" style="59" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="59" customWidth="1"/>
-    <col min="7" max="12" width="5.42578125" style="59" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="3.83203125" style="59" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" style="59" customWidth="1"/>
+    <col min="4" max="4" width="42.5" style="59" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="59" customWidth="1"/>
+    <col min="7" max="12" width="5.5" style="59" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21"/>
       <c r="B1" s="22" t="s">
         <v>83</v>
@@ -6521,7 +6723,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="2" spans="1:12" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -6535,7 +6737,7 @@
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
     </row>
-    <row r="3" spans="1:12" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="214" t="s">
         <v>9</v>
       </c>
@@ -6563,7 +6765,7 @@
       <c r="K3" s="216"/>
       <c r="L3" s="217"/>
     </row>
-    <row r="4" spans="1:12" s="30" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="30" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="215"/>
       <c r="B4" s="213"/>
       <c r="C4" s="213"/>
@@ -6589,7 +6791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="38" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="38" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="31">
         <v>1</v>
       </c>
@@ -6627,7 +6829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="38" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="38" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="31">
         <v>2</v>
       </c>
@@ -6665,7 +6867,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="38" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="38" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A7" s="31">
         <v>3</v>
       </c>
@@ -6701,7 +6903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="38" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="38" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="31">
         <v>4</v>
       </c>
@@ -6739,7 +6941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="38" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="38" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="31">
         <v>5</v>
       </c>
@@ -6773,7 +6975,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="38" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="38" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="31">
         <v>6</v>
       </c>
@@ -6809,7 +7011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="38" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="38" customFormat="1" ht="108" x14ac:dyDescent="0.15">
       <c r="A11" s="31">
         <v>7</v>
       </c>
@@ -6845,7 +7047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="38" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="38" customFormat="1" ht="144" x14ac:dyDescent="0.15">
       <c r="A12" s="31">
         <v>8</v>
       </c>
@@ -6881,7 +7083,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="38" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="38" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="31">
         <v>9</v>
       </c>
@@ -6917,7 +7119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="38" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="38" customFormat="1" ht="168" x14ac:dyDescent="0.15">
       <c r="A14" s="31">
         <v>10</v>
       </c>
@@ -6955,7 +7157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="38" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="38" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="31">
         <v>11</v>
       </c>
@@ -6993,7 +7195,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="38" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="38" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="31">
         <v>12</v>
       </c>
@@ -7031,7 +7233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="38" customFormat="1" ht="189" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="38" customFormat="1" ht="189" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="31">
         <v>13</v>
       </c>
@@ -7063,7 +7265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="38" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="38" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="31">
         <v>14</v>
       </c>
@@ -7101,7 +7303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="44" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="44" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="39">
         <v>15</v>
       </c>
@@ -7133,7 +7335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="38" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="38" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="45">
         <v>16</v>
       </c>
@@ -7165,7 +7367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="38" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="38" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="39">
         <v>17</v>
       </c>
@@ -7197,7 +7399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="38" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="38" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="45">
         <v>18</v>
       </c>
@@ -7229,7 +7431,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="38" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="38" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="39">
         <v>19</v>
       </c>
@@ -7259,7 +7461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="38" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="38" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="45">
         <v>20</v>
       </c>
@@ -7291,7 +7493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="38" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="38" customFormat="1" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" s="39">
         <v>21</v>
       </c>
@@ -7321,7 +7523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="38" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="38" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="45">
         <v>22</v>
       </c>
@@ -7349,7 +7551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="38" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="38" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="39">
         <v>23</v>
       </c>
@@ -7379,7 +7581,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="38" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="38" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="45">
         <v>24</v>
       </c>
@@ -7407,7 +7609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="38" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="38" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="39">
         <v>25</v>
       </c>
@@ -7437,7 +7639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="38" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" s="38" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="45">
         <v>26</v>
       </c>
@@ -7465,7 +7667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A31" s="39">
         <v>27</v>
       </c>
@@ -7495,7 +7697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="38" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" s="38" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="45">
         <v>28</v>
       </c>
@@ -7529,7 +7731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="38" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="38" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="39">
         <v>29</v>
       </c>
@@ -7563,7 +7765,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="38" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="38" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="45">
         <v>30</v>
       </c>
@@ -7593,7 +7795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="38" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" s="38" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="39">
         <v>31</v>
       </c>
@@ -7619,7 +7821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="38" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" s="38" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="45">
         <v>32</v>
       </c>
@@ -7649,7 +7851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="38" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" s="38" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="39">
         <v>33</v>
       </c>
@@ -7683,7 +7885,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="38" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="38" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="51">
         <v>34</v>
       </c>
@@ -7711,153 +7913,153 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E39" s="27"/>
     </row>
-    <row r="40" spans="1:12" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="58" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E40" s="27"/>
     </row>
-    <row r="41" spans="1:12" s="58" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" s="58" customFormat="1" x14ac:dyDescent="0.15">
       <c r="E41" s="27"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" s="58"/>
       <c r="B42" s="16"/>
       <c r="C42" s="17"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B43" s="16"/>
       <c r="C43" s="17"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B44" s="16"/>
       <c r="C44" s="17"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B45" s="16"/>
       <c r="C45" s="17"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B46" s="16"/>
       <c r="C46" s="17"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B47" s="16"/>
       <c r="C47" s="17"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B48" s="16"/>
       <c r="C48" s="17"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B49" s="16"/>
       <c r="C49" s="17"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B50" s="61"/>
       <c r="C50" s="17"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B51" s="61"/>
       <c r="C51" s="17"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B52" s="61"/>
       <c r="C52" s="17"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B53" s="61"/>
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B54" s="61"/>
       <c r="C54" s="17"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B55" s="61"/>
       <c r="C55" s="17"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B56" s="61"/>
       <c r="C56" s="17"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B57" s="61"/>
       <c r="C57" s="17"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B58" s="61"/>
       <c r="C58" s="17"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B59" s="61"/>
       <c r="C59" s="17"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B60" s="61"/>
       <c r="C60" s="17"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B61" s="61"/>
       <c r="C61" s="17"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B62" s="61"/>
       <c r="C62" s="17"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B63" s="61"/>
       <c r="C63" s="17"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B64" s="61"/>
       <c r="C64" s="17"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B65" s="61"/>
       <c r="C65" s="17"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B66" s="61"/>
       <c r="C66" s="17"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B67" s="61"/>
       <c r="C67" s="17"/>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B68" s="61"/>
       <c r="C68" s="17"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B69" s="61"/>
       <c r="C69" s="17"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B70" s="61"/>
       <c r="C70" s="17"/>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B71" s="61"/>
       <c r="C71" s="17"/>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B72" s="61"/>
       <c r="C72" s="17"/>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B73" s="61"/>
       <c r="C73" s="17"/>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B74" s="61"/>
       <c r="C74" s="17"/>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B75" s="61"/>
       <c r="C75" s="17"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B76" s="61"/>
       <c r="C76" s="17"/>
     </row>
@@ -7942,20 +8144,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Priority xmlns="41A7A25E-88C5-415C-AB9A-358CCBEA8A85" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Priority xmlns="41A7A25E-88C5-415C-AB9A-358CCBEA8A85" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7976,6 +8178,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DAA1354-1B65-433B-8B6C-AAF4E176B712}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4C8E2CD-F38F-41D1-821F-079AD38244FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -7989,12 +8199,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8DAA1354-1B65-433B-8B6C-AAF4E176B712}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>